<commit_message>
Add Fitur Transaksi Pemesanan ke Bill
</commit_message>
<xml_diff>
--- a/src/data/dataBill.xlsx
+++ b/src/data/dataBill.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Nama</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Quantity</t>
   </si>
@@ -35,7 +32,16 @@
     <t>Harga</t>
   </si>
   <si>
-    <t>a</t>
+    <t>Resto</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Oto Bento</t>
+  </si>
+  <si>
+    <t>Chicken Blackpepper</t>
   </si>
 </sst>
 </file>
@@ -353,34 +359,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2">
+        <v>25000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error di waiting display waktu nulis ke file transaksi per toko sama di dashboard waktu ngitung datanya
</commit_message>
<xml_diff>
--- a/src/data/dataBill.xlsx
+++ b/src/data/dataBill.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regawa\Documents\NetBeansProjects\NEWPROYEK2\FoodCourt\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\NetBeansProjects\FoodCourt2\FoodCourt\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowHeight="7760" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,30 +24,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Harga</t>
-  </si>
-  <si>
-    <t>Resto</t>
-  </si>
-  <si>
-    <t>Menu</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+  <si>
+    <t>toko</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>harga</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>Beef Spaghetti</t>
+  </si>
+  <si>
+    <t>Cheesy Melt Potato</t>
+  </si>
+  <si>
+    <t>Han Gang</t>
+  </si>
+  <si>
+    <t>Jab-chae</t>
   </si>
   <si>
     <t>Oto Bento</t>
   </si>
   <si>
-    <t>Chicken Blackpepper</t>
+    <t>Nasi Putih</t>
+  </si>
+  <si>
+    <t>Chicken Fried Rice</t>
+  </si>
+  <si>
+    <t>Chicken Baaga</t>
+  </si>
+  <si>
+    <t>Arasseo</t>
+  </si>
+  <si>
+    <t>Wild Wild Wings</t>
+  </si>
+  <si>
+    <t>Ojingeo Bokeum</t>
+  </si>
+  <si>
+    <t>Kacamata</t>
+  </si>
+  <si>
+    <t>Nasi Hainam Chasiu Siobak</t>
+  </si>
+  <si>
+    <t>Ootoya</t>
+  </si>
+  <si>
+    <t>Gokoku Gohan</t>
+  </si>
+  <si>
+    <t>Kyochon</t>
+  </si>
+  <si>
+    <t>Mineral Water</t>
+  </si>
+  <si>
+    <t>Ayam Bakar Ganthari</t>
+  </si>
+  <si>
+    <t>Aqua</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,16 +130,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -101,10 +156,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -139,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,7 +229,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,21 +323,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -299,7 +354,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -351,55 +406,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>25000</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
read/write transaksi - bill oke!
</commit_message>
<xml_diff>
--- a/src/data/dataBill.xlsx
+++ b/src/data/dataBill.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>toko</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Aqua</t>
+  </si>
+  <si>
+    <t>Short Ribs</t>
+  </si>
+  <si>
+    <t>Arasseo Steak Tartara</t>
+  </si>
+  <si>
+    <t>Chicken Katsu Rice</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Pada modul button print bill
</commit_message>
<xml_diff>
--- a/src/data/dataBill.xlsx
+++ b/src/data/dataBill.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
   <si>
     <t>toko</t>
   </si>
@@ -105,6 +105,57 @@
   </si>
   <si>
     <t>Chicken Katsu Rice</t>
+  </si>
+  <si>
+    <t>Chicken Teriyaki</t>
+  </si>
+  <si>
+    <t>Juice Jambu</t>
+  </si>
+  <si>
+    <t>Beef Fettuccine</t>
+  </si>
+  <si>
+    <t>Creamy Chicken Baked Rice</t>
+  </si>
+  <si>
+    <t>Aqua 330 mL</t>
+  </si>
+  <si>
+    <t>Nasi Hainam Siobak</t>
+  </si>
+  <si>
+    <t>Bakmi Hongkong Chasiu Siobak</t>
+  </si>
+  <si>
+    <t>Lemon Tea</t>
+  </si>
+  <si>
+    <t>Green Tea</t>
+  </si>
+  <si>
+    <t>Nasi Hainam Campur</t>
+  </si>
+  <si>
+    <t>Air Mineral Botol</t>
+  </si>
+  <si>
+    <t>Cincau</t>
+  </si>
+  <si>
+    <t>Nasi Hainam Polos</t>
+  </si>
+  <si>
+    <t>Bakmi Hongkong Chasiu</t>
+  </si>
+  <si>
+    <t>Nasi Putih Bebek</t>
+  </si>
+  <si>
+    <t>Bakmi Hongkong Siobak</t>
+  </si>
+  <si>
+    <t>Susu Kacang</t>
   </si>
 </sst>
 </file>
@@ -423,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -450,6 +501,62 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>54450.00000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>52030.00000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>18150.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>18150.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Relayout Integrasi, Passing no meja
</commit_message>
<xml_diff>
--- a/src/data/dataBill.xlsx
+++ b/src/data/dataBill.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>toko</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Susu Kacang</t>
+  </si>
+  <si>
+    <t>Chicken Blackpepper</t>
+  </si>
+  <si>
+    <t>Fresh Salad</t>
+  </si>
+  <si>
+    <t>Fresh Girl</t>
   </si>
 </sst>
 </file>
@@ -474,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -501,62 +510,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>54450.00000000001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>52030.00000000001</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>18150.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>18150.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>